<commit_message>
add function: add the detail information about the interface introduction of excel
</commit_message>
<xml_diff>
--- a/生成excel表格-自动填充-设置颜色/测试.xlsx
+++ b/生成excel表格-自动填充-设置颜色/测试.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code data\Powershell\生成excel表格-自动填充-设置颜色\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC73FE6B-D0F4-4E59-AAD8-DBB2F3FCD94E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A184AF19-6407-498E-A713-C80482C6E7CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3468" yWindow="1932" windowWidth="17280" windowHeight="8964" xr2:uid="{0B7EBB33-37A0-4269-96E8-81E540A55716}"/>
+    <workbookView xWindow="3468" yWindow="1932" windowWidth="17280" windowHeight="8964" xr2:uid="{80248D26-90D8-43CA-893C-D77114E9D1BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Processes" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA2E056E-F2DA-4765-BE22-0A2AAD25B89A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A877BE-2806-4D19-A9A3-E4A000D80257}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -489,25 +489,25 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>4915200</v>
+        <v>3903488</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3">
-        <v>5271552</v>
+        <v>4063232</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4">
-        <v>4919296</v>
+        <v>3932160</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5">
-        <v>65544192</v>
+        <v>62607360</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -515,7 +515,7 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>17461248</v>
+        <v>16486400</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -523,7 +523,7 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>9330688</v>
+        <v>21458944</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -531,7 +531,7 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>53104640</v>
+        <v>50139136</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -539,7 +539,7 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>118575104</v>
+        <v>110174208</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -547,7 +547,7 @@
         <v>2</v>
       </c>
       <c r="B10">
-        <v>27856896</v>
+        <v>14221312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>